<commit_message>
kleine aanpassing in table 1 en code
</commit_message>
<xml_diff>
--- a/table 1.xlsx
+++ b/table 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f5275acbae45a446/Documenten/2021-2022/semester 2/bachelorproject/our-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="210" documentId="8_{70F01EE1-9D1F-4316-996A-9CCBE6EB023D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C57F210-8B9D-4FC9-9D8F-B5834508366F}"/>
+  <xr:revisionPtr revIDLastSave="212" documentId="8_{70F01EE1-9D1F-4316-996A-9CCBE6EB023D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B745F04A-A81E-48C0-9343-213D5CB5B386}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BE625CA8-5B1C-4F5B-923D-A7F559D93353}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="63">
   <si>
     <t>White/Hispanic</t>
   </si>
@@ -221,6 +221,9 @@
   </si>
   <si>
     <t>[2,67]</t>
+  </si>
+  <si>
+    <t>None (6)</t>
   </si>
 </sst>
 </file>
@@ -271,9 +274,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -281,6 +281,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -611,16 +614,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1" t="s">
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
@@ -639,552 +642,557 @@
         <v>6</v>
       </c>
       <c r="G2" t="s">
-        <v>4</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>26.553000000000001</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>52.13</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>35.591999999999999</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
         <v>24.004999999999999</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="2">
         <v>32.47</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="2">
         <v>25.98</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>27.56</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>41.881999999999998</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <v>35.901000000000003</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>26.01</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="2">
         <v>28.94</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="2">
         <v>24.164000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="3">
         <v>0.50800000000000001</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <v>0.18</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <v>0.42199999999999999</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="3">
         <v>0.33300000000000002</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="3">
         <v>0.20100000000000001</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="3">
         <v>0.377</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="3" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="3">
         <v>0.53300000000000003</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="3">
         <v>0.248</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="3">
         <v>0.41</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="3">
         <v>0.38800000000000001</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="3">
         <v>0.27100000000000002</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="3">
         <v>0.36699999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="3" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
+      <c r="A12" s="1"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="3">
         <v>0.22</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="3">
         <v>0.40500000000000003</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="3">
         <v>0.22800000000000001</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="3">
         <v>0.313</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F13" s="3">
         <v>0.502</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13" s="3">
         <v>0.27800000000000002</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="A14" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F14" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="G14" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="A15" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="3">
         <v>0.16200000000000001</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="3">
         <v>0.308</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="3">
         <v>0.216</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="3">
         <v>0.316</v>
       </c>
-      <c r="F15" s="4">
+      <c r="F15" s="3">
         <v>0.42399999999999999</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G15" s="3">
         <v>0.29699999999999999</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F16" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G16" s="4" t="s">
+      <c r="G16" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
+      <c r="A17" s="1"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="A18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="3">
         <v>-0.442</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="3">
         <v>0.23300000000000001</v>
       </c>
-      <c r="D18" s="4">
+      <c r="D18" s="3">
         <v>-0.214</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="3">
         <v>-0.751</v>
       </c>
-      <c r="F18" s="4">
+      <c r="F18" s="3">
         <v>-0.51400000000000001</v>
       </c>
-      <c r="G18" s="4">
+      <c r="G18" s="3">
         <v>-0.67600000000000005</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="A19" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F19" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G19" s="4" t="s">
+      <c r="G19" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="A20" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B20" s="3">
         <v>-0.47599999999999998</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20" s="3">
         <v>1.77E-2</v>
       </c>
-      <c r="D20" s="4">
+      <c r="D20" s="3">
         <v>-0.20100000000000001</v>
       </c>
-      <c r="E20" s="4">
+      <c r="E20" s="3">
         <v>-0.77400000000000002</v>
       </c>
-      <c r="F20" s="4">
+      <c r="F20" s="3">
         <v>-0.627</v>
       </c>
-      <c r="G20" s="4">
+      <c r="G20" s="3">
         <v>-0.76100000000000001</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="A21" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E21" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F21" s="4" t="s">
+      <c r="F21" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="G21" s="4" t="s">
+      <c r="G21" s="3" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
+      <c r="A22" s="1"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="A23" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="4">
+      <c r="B23" s="3">
         <v>8.5299999999999994</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C23" s="4">
         <v>10.6</v>
       </c>
-      <c r="D23" s="4">
+      <c r="D23" s="3">
         <v>9.34</v>
       </c>
-      <c r="E23" s="4">
+      <c r="E23" s="3">
         <v>9.7100000000000009</v>
       </c>
-      <c r="F23" s="5">
+      <c r="F23" s="4">
         <v>10.9</v>
       </c>
-      <c r="G23" s="4">
+      <c r="G23" s="3">
         <v>9.6999999999999993</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="A24" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D24" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="E24" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F24" s="4" t="s">
+      <c r="F24" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="G24" s="4" t="s">
+      <c r="G24" s="3" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="A25" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="4">
+      <c r="B25" s="3">
         <v>8.51</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C25" s="4">
         <v>10.1</v>
       </c>
-      <c r="D25" s="4">
+      <c r="D25" s="3">
         <v>9.5399999999999991</v>
       </c>
-      <c r="E25" s="4">
+      <c r="E25" s="3">
         <v>9.82</v>
       </c>
-      <c r="F25" s="5">
+      <c r="F25" s="4">
         <v>10.1</v>
       </c>
-      <c r="G25" s="4">
+      <c r="G25" s="3">
         <v>9.98</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="A26" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D26" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E26" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="F26" s="4" t="s">
+      <c r="F26" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="G26" s="4" t="s">
+      <c r="G26" s="3" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+      <c r="A28" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B28" s="2">
+      <c r="B28" s="1">
         <v>364</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28" s="1">
         <v>745</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D28" s="1">
         <v>1374</v>
       </c>
-      <c r="E28" s="2">
+      <c r="E28" s="1">
         <v>415</v>
       </c>
-      <c r="F28" s="2">
+      <c r="F28" s="1">
         <v>249</v>
       </c>
-      <c r="G28" s="2">
+      <c r="G28" s="1">
         <v>551</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+      <c r="A29" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B29" s="1">
         <v>229</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="1">
         <v>315</v>
       </c>
-      <c r="D29" s="2">
+      <c r="D29" s="1">
         <v>510</v>
       </c>
-      <c r="E29" s="2">
+      <c r="E29" s="1">
         <v>206</v>
       </c>
-      <c r="F29" s="2">
+      <c r="F29" s="1">
         <v>144</v>
       </c>
-      <c r="G29" s="2">
+      <c r="G29" s="1">
         <v>259</v>
       </c>
     </row>

</xml_diff>